<commit_message>
updated Bug Metrics.docx and Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/testing/Test Cases.xlsx
+++ b/testing/Test Cases.xlsx
@@ -685,6 +685,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,18 +722,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,56 +1067,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="24" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="29"/>
-      <c r="O1" s="30" t="s">
+      <c r="N1" s="33"/>
+      <c r="O1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="32" t="s">
+      <c r="P1" s="35"/>
+      <c r="Q1" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="32"/>
+      <c r="R1" s="36"/>
     </row>
     <row r="2" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1476,8 +1476,8 @@
       <c r="K10" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="L10" s="19" t="s">
-        <v>29</v>
+      <c r="L10" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
@@ -2260,6 +2260,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -2267,11 +2272,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>